<commit_message>
Fixed salary order in JOGI
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
+++ b/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\github\python_project-dataset\Files\college_info\all_colleges\JOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860A4B82-C191-4F95-919F-E1950E97C1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C294E7-E84B-4A1B-AB0B-C523CBC4BDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$14</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -474,7 +477,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -503,14 +506,14 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>3.36</v>
+        <v>3.5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
@@ -518,13 +521,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1">
@@ -545,14 +548,14 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>3.36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
@@ -574,27 +577,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.25" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
-        <v>2.87</v>
+        <v>3.25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1">
@@ -602,13 +605,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="31.5" customHeight="1" thickBot="1">
@@ -616,13 +619,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>3.25</v>
+        <v>2.87</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
@@ -630,13 +633,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>2.75</v>
+        <v>2.87</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1">
@@ -644,13 +647,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
-        <v>2.57</v>
+        <v>2.75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
@@ -658,13 +661,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>2.87</v>
+        <v>2.75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1">
@@ -672,16 +675,21 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>2.75</v>
+        <v>2.57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:D14" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D14">
+      <sortCondition descending="1" ref="C1:C14"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the bug in jogi
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
+++ b/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
@@ -1,71 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\github\python_project-dataset\Files\college_info\all_colleges\JOGI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\gitt\PYTHON PROJECT\github\python_project-dataset\Files\college_info\all_colleges\JOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C294E7-E84B-4A1B-AB0B-C523CBC4BDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DA03D1-0286-46A3-85AD-2AE52234F6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
-  <si>
-    <t>8   </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Tata Consulting Services</t>
   </si>
   <si>
-    <t>1   </t>
-  </si>
-  <si>
     <t>WIPRO</t>
   </si>
   <si>
     <t>COGNIZANT</t>
   </si>
   <si>
-    <t>14   </t>
-  </si>
-  <si>
     <t>Miraki Tech</t>
   </si>
   <si>
-    <t>2   </t>
-  </si>
-  <si>
     <t>KTREE</t>
   </si>
   <si>
-    <t>7   </t>
-  </si>
-  <si>
     <t>Legato Health   Technologies</t>
   </si>
   <si>
-    <t>23   </t>
-  </si>
-  <si>
     <t>Insmagro Global   Solutions Pvt Ltd</t>
   </si>
   <si>
@@ -75,25 +67,13 @@
     <t>PragmaEdge software   services private limited</t>
   </si>
   <si>
-    <t>9   </t>
-  </si>
-  <si>
     <t>QSPIDERS</t>
   </si>
   <si>
-    <t>16   </t>
-  </si>
-  <si>
     <t>Euthissa</t>
   </si>
   <si>
-    <t>12   </t>
-  </si>
-  <si>
     <t>Aliens Group</t>
-  </si>
-  <si>
-    <t>6   </t>
   </si>
   <si>
     <t>Packet prep</t>
@@ -183,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -194,6 +174,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,141 +458,140 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="28.2" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>3.5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D3" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>3.38</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>3.36</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>3.25</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>3.25</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29.25" thickBot="1">
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.2" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>3.25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
+      <c r="D9" s="4">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="31.5" customHeight="1" thickBot="1">
@@ -619,74 +599,74 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
         <v>2.87</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D10" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>2.87</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D11" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
         <v>2.75</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D12" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>2.75</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
         <v>2.57</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
+      <c r="D14" s="4">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D14" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D14">
+  <autoFilter ref="B1:C14" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C14">
       <sortCondition descending="1" ref="C1:C14"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added placement analysis to srikar colleges
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
+++ b/Files/college_info/all_colleges/JOGI/JOGI_placements.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\gitt\PYTHON PROJECT\github\python_project-dataset\Files\college_info\all_colleges\JOGI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Arshad Ali\Dropbox\Programming\KMIT\Projects\group\python project on dataset (1st year 2nd sem)\files\all_colleges\JOGI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DA03D1-0286-46A3-85AD-2AE52234F6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBCCE4-348D-4773-B7EE-2EE0F7CA2888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$14</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -95,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +108,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,15 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -458,7 +443,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -468,17 +453,17 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -492,7 +477,7 @@
       <c r="C2" s="1">
         <v>3.5</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -506,7 +491,7 @@
       <c r="C3" s="1">
         <v>3.5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>7</v>
       </c>
     </row>
@@ -520,7 +505,7 @@
       <c r="C4" s="1">
         <v>3.38</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -534,7 +519,7 @@
       <c r="C5" s="1">
         <v>3.36</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>8</v>
       </c>
     </row>
@@ -548,7 +533,7 @@
       <c r="C6" s="1">
         <v>3.25</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
     </row>
@@ -562,7 +547,7 @@
       <c r="C7" s="1">
         <v>3.25</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -576,7 +561,7 @@
       <c r="C8" s="1">
         <v>3.25</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>2</v>
       </c>
     </row>
@@ -590,7 +575,7 @@
       <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>14</v>
       </c>
     </row>
@@ -604,7 +589,7 @@
       <c r="C10" s="1">
         <v>2.87</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>23</v>
       </c>
     </row>
@@ -618,7 +603,7 @@
       <c r="C11" s="1">
         <v>2.87</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>112</v>
       </c>
     </row>
@@ -632,7 +617,7 @@
       <c r="C12" s="1">
         <v>2.75</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>9</v>
       </c>
     </row>
@@ -646,7 +631,7 @@
       <c r="C13" s="1">
         <v>2.75</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>6</v>
       </c>
     </row>
@@ -660,16 +645,11 @@
       <c r="C14" s="1">
         <v>2.57</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C14" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C14">
-      <sortCondition descending="1" ref="C1:C14"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>